<commit_message>
adding correlations, fixed the discretized attempts bug
</commit_message>
<xml_diff>
--- a/_site/tables_for_blog.xlsx
+++ b/_site/tables_for_blog.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamarnesen/Documents/SizingBlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795B51A7-9671-7746-ABC6-E41FD5DD1114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E7A3B2-CD92-904E-95CD-9B6A0A38149E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11000" yWindow="820" windowWidth="15180" windowHeight="17440" activeTab="2" xr2:uid="{1308396A-5B64-0148-815D-B4C4DFC62E83}"/>
+    <workbookView xWindow="15060" yWindow="820" windowWidth="15180" windowHeight="17440" activeTab="3" xr2:uid="{1308396A-5B64-0148-815D-B4C4DFC62E83}"/>
   </bookViews>
   <sheets>
     <sheet name="SimpleProb" sheetId="1" r:id="rId1"/>
     <sheet name="DiscountedProb" sheetId="2" r:id="rId2"/>
     <sheet name="HurdleRates" sheetId="3" r:id="rId3"/>
+    <sheet name="Variable Definitions" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Phase</t>
   </si>
@@ -95,6 +96,36 @@
   </si>
   <si>
     <t>Funder's present value of payout</t>
+  </si>
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>$/theta$</t>
+  </si>
+  <si>
+    <t>$n$</t>
+  </si>
+  <si>
+    <t>$p$</t>
+  </si>
+  <si>
+    <t>Per-attempt probability of success</t>
+  </si>
+  <si>
+    <t>Number of attempts</t>
+  </si>
+  <si>
+    <t>Target probability of success</t>
+  </si>
+  <si>
+    <t>$X$</t>
+  </si>
+  <si>
+    <t>Present value of pull size</t>
   </si>
 </sst>
 </file>
@@ -795,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2116782-64C9-1349-AF7E-D9C428D36E5E}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -866,5 +897,61 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FD9408-0C5A-D342-B67D-779865230ACA}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>